<commit_message>
HW_3 completed, with quite good lined ROC (via ML result)
</commit_message>
<xml_diff>
--- a/src/main/reports/Report.xlsx
+++ b/src/main/reports/Report.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ML Logistic Regression Model" sheetId="1" r:id="rId1"/>
     <sheet name="ROC" sheetId="2" r:id="rId2"/>
+    <sheet name="ROC (via ML)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Number of features used</t>
   </si>
@@ -675,7 +676,1863 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ROC (via ML)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'ROC (via ML)'!$A$2:$A$1508</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1507"/>
+                <c:pt idx="0">
+                  <c:v>3.7174721189590998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6914498141263899E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6654275092936792E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.41263940520446E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8587360594795502E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2304832713754601E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.60223048327137E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8996282527881001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.27137546468401E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5687732342007401E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7918215613382898E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2379182156133802E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4609665427509201E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7583643122676503E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.2044609665427503E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.65055762081784E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0966542750929303E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4684014869888395E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.9144981412639403E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.2862453531598495E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.7323420074349405E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.1784386617100302E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.5501858736059394E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.9962825278810402E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.3680297397769494E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.8141263940520404E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.101115241635687</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.10334572490706299</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.10557620817843801</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.109293680297397</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.112267657992565</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.116728624535315</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.121189591078066</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.12416356877323401</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.12788104089219299</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.131598513011152</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.13457249070631899</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.136802973977695</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.139776951672862</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.14423791821561299</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.147955390334572</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.15018587360594701</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.15315985130111501</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.15687732342007399</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.15985130111524101</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.16431226765799201</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.16802973977695099</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.17249070631970201</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.176951672862453</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.18066914498141201</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.185130111524163</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.18884758364312201</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.19182156133828901</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.19628252788104</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.199256505576208</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.20297397769516701</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.20669144981412599</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.21115241635687701</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.215613382899628</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.21933085501858701</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.22304832713754599</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.226765799256505</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.23048327137546401</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.234944237918215</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.239405204460966</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.24237918215613299</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.246096654275092</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.24981412639405201</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.25353159851301099</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.25799256505576201</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.26245353159851298</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.26542750929367998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.269888475836431</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.27360594795539001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.27732342007434901</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.28178438661709998</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.286245353159851</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.29070631970260202</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.29516728624535299</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.29814126394051998</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.30185873605947899</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.30631970260223002</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.31078066914498098</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.31449814126393999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.31895910780669101</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.32342007434944198</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.327881040892193</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.33159851301115201</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.33531598513011102</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.33977695167286198</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.344237918215613</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.34795539033457201</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.35167286245353102</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.35613382899628199</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.36059479553903301</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.36282527881040799</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.366542750929368</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.37026022304832701</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.37397769516728602</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.37843866171003698</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.38066914498141202</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.38438661710037098</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.388847583643122</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.39256505576208101</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.395539033457249</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.398513011152416</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.40297397769516702</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.40594795539033401</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.40966542750929302</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.41263940520446002</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.41710037174721099</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.42156133828996201</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.42602230483271297</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.43048327137546399</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.43345724907063199</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.437174721189591</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.44163568773234202</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.44609665427509199</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.45055762081784301</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.45501858736059397</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.45947955390334499</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.463197026022304</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.46691449814126301</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.47063197026022302</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.47434944237918197</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.47657992565055701</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.48104089219330798</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.48475836431226699</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.48921933085501801</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.49293680297397702</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.49739776951672798</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.50037174721189503</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.504832713754646</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.50929368029739697</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.51375464684014804</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.51821561338289901</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.52193308550185802</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.52565055762081703</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.52936802973977604</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.533828996282527</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.53828996282527797</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.54275092936802904</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.54721189591078001</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.55092936802973902</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.55464684014869803</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.55836431226765804</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.562825278810408</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.56728624535315897</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.57100371747211898</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.57472118959107799</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.57918215613382895</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.58289962825278796</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.58736059479553904</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.59182156133829</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.59553903345724901</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.59925650557620802</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.60297397769516703</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.607434944237918</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.61189591078066896</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.61561338289962797</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.61933085501858698</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.62379182156133794</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.62825278810408902</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.63271375464683999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.636431226765799</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.64089219330854996</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.64535315985130104</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.64981412639405201</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.65353159851301101</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.65724907063197002</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.66171003717472099</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.66542750929368</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.66914498141263901</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.67360594795538997</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.67806691449814105</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.68252788104089201</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.68698884758364298</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.69070631970260199</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.694423791821561</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.69888475836431196</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.70334572490706304</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.70780669144981401</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.71226765799256497</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.71598513011152398</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.72044609665427495</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.723420074349442</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.72788104089219297</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.73234200743494404</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.73680297397769501</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.73977695167286195</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.74423791821561303</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.74869888475836399</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.75315985130111496</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.75687732342007397</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.76133828996282504</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.76505576208178405</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.76951672862453502</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.77397769516728598</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.77769516728624499</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.781412639405204</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.78587360594795497</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.79033457249070604</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.79479553903345701</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.79925650557620798</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.80371747211895905</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.80743494423791795</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.81189591078066903</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.81635687732341999</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.82081784386617096</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.82527881040892104</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.82899628252788105</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.83345724907063201</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.83717472118959102</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.84163568773234199</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.84609665427509295</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.84981412639405196</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.85427509293680204</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.858736059479553</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.86319702602230397</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.86691449814126398</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.87063197026022299</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.874349442379182</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.878066914498141</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.88178438661710001</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.88624535315985098</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.89070631970260195</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.89516728624535302</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.89962825278810399</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.903345724907063</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.90780669144981396</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.91226765799256504</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.91672862453531601</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.92118959107806597</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.92565055762081705</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.92936802973977695</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.93382899628252702</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.93828996282527799</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.94275092936802896</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.94721189591078003</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.951672862453531</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.95613382899628196</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.96059479553903304</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.96505576208178401</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.96951672862453497</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.97323420074349398</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.97769516728624495</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.98215613382899603</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.98661710037174699</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.98959107806691404</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.99405204460966501</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.99851301115241597</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'ROC (via ML)'!$B$2:$B$1508</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1507"/>
+                <c:pt idx="0">
+                  <c:v>6.13496932515337E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.84049079754601E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0674846625766802E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0674846625766802E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0674846625766802E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6809815950920199E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2944785276073601E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5214723926380299E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.13496932515337E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3619631901840496E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2024539877300596E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2024539877300596E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11042944785276</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.122699386503067</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.122699386503067</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.122699386503067</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.122699386503067</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.12883435582822</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.12883435582822</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.13496932515337401</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13496932515337401</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.13496932515337401</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.14110429447852699</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.14110429447852699</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.14723926380368099</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.14723926380368099</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.159509202453987</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.17791411042944699</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.19631901840490701</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.20245398773006101</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.214723926380368</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.214723926380368</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.214723926380368</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.22699386503067401</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.23312883435582801</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.23926380368098099</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.251533742331288</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.26993865030674802</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.28220858895705497</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.28220858895705497</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.28834355828220798</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.306748466257668</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.31901840490797501</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.32515337423312801</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.33742331288343502</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.33742331288343502</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.34355828220858797</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.34355828220858797</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.34355828220858797</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.34969325153374198</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.34969325153374198</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.35582822085889498</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.36809815950920199</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.36809815950920199</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.380368098159509</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.38650306748466201</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.39263803680981502</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.39263803680981502</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.39263803680981502</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.39877300613496902</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.40490797546012203</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.41104294478527598</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.41717791411042898</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.41717791411042898</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.41717791411042898</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.42944785276073599</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.435582822085889</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.441717791411042</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.44785276073619601</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.44785276073619601</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.44785276073619601</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.46012269938650302</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.46012269938650302</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.46625766871165603</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.47239263803680898</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.47239263803680898</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.47239263803680898</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.47239263803680898</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.47239263803680898</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.48466257668711599</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.49079754601226899</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.49079754601226899</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.49079754601226899</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.496932515337423</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.496932515337423</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.496932515337423</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.496932515337423</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.503067484662576</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.50920245398773001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.50920245398773001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.50920245398773001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.51533742331288301</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.52147239263803602</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.52147239263803602</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.52147239263803602</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.53987730061349604</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.54601226993865004</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.55214723926380305</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.55828220858895705</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.55828220858895705</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.57668711656441696</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.58282208588956996</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.58282208588956996</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.58895705521472397</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.60122699386502998</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.61349693251533699</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.61349693251533699</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.625766871165644</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.63190184049079701</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.64417177914110402</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.64417177914110402</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.64417177914110402</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.64417177914110402</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.64417177914110402</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.65644171779141103</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.66257668711656403</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.66257668711656403</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.66257668711656403</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.66257668711656403</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.66257668711656403</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.66257668711656403</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.66871165644171704</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.67484662576687104</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.68098159509202405</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.68711656441717694</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.70552147239263796</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.70552147239263796</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.71165644171779097</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.71165644171779097</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.71779141104294397</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.71779141104294397</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.73006134969325098</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.73006134969325098</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.73006134969325098</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.73006134969325098</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.73006134969325098</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.73619631901840399</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.74233128834355799</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.748466257668711</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.748466257668711</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.748466257668711</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.748466257668711</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.748466257668711</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.754601226993865</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.76073619631901801</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.76687116564417102</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.76687116564417102</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.76687116564417102</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.77300613496932502</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.77914110429447803</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.77914110429447803</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.78527607361963103</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.78527607361963103</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.78527607361963103</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.79141104294478504</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.79754601226993804</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.80368098159509205</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.80368098159509205</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.80368098159509205</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.80981595092024505</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.81595092024539795</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.81595092024539795</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.81595092024539795</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.81595092024539795</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.82208588957055195</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.82208588957055195</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.82208588957055195</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.82208588957055195</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.82822085889570496</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.83435582822085796</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.83435582822085796</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.84049079754601197</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.84662576687116498</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.84662576687116498</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.84662576687116498</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.84662576687116498</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.84662576687116498</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.85276073619631898</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.85889570552147199</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.85889570552147199</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.85889570552147199</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.85889570552147199</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.85889570552147199</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.86503067484662499</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.86503067484662499</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.877300613496932</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.877300613496932</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.877300613496932</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.877300613496932</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.88957055214723901</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.88957055214723901</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.88957055214723901</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.88957055214723901</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.89570552147239202</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.89570552147239202</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.90184049079754602</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.90184049079754602</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.90184049079754602</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.90797546012269903</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.91411042944785204</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.91411042944785204</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.91411042944785204</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.91411042944785204</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.91411042944785204</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.91411042944785204</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.92024539877300604</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.92024539877300604</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.92024539877300604</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.92024539877300604</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.92024539877300604</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.92638036809815905</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.92638036809815905</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.93251533742331205</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.93251533742331205</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.93251533742331205</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.93865030674846595</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.93865030674846595</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.93865030674846595</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.93865030674846595</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.94478527607361895</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.95092024539877296</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.95705521472392596</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.96319018404907897</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.96932515337423297</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.96932515337423297</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.96932515337423297</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.96932515337423297</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.96932515337423297</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.97546012269938598</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.97546012269938598</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.97546012269938598</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.97546012269938598</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.97546012269938598</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.97546012269938598</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.98159509202453898</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.98773006134969299</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.98773006134969299</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.98773006134969299</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.98773006134969299</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B3FF-455C-862E-1B717C09ED12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'ROC (via ML)'!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'ROC (via ML)'!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B3FF-455C-862E-1B717C09ED12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1636932064"/>
+        <c:axId val="1636918752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1636932064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1636918752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1636918752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1636932064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1231,6 +3088,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1249,6 +3622,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2058,8 +4466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1509"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14261,4 +16669,2060 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D253"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>3.7174721189590998E-3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.13496932515337E-3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>6.6914498141263899E-3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.84049079754601E-2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>9.6654275092936792E-3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.0674846625766802E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.41263940520446E-2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3.0674846625766802E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.8587360594795502E-2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.0674846625766802E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2.2304832713754601E-2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.6809815950920199E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2.60223048327137E-2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.2944785276073601E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.8996282527881001E-2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.5214723926380299E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3.27137546468401E-2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6.13496932515337E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3.5687732342007401E-2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.3619631901840496E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>3.7918215613382898E-2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9.2024539877300596E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4.2379182156133802E-2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9.2024539877300596E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4.4609665427509201E-2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.11042944785276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>4.7583643122676503E-2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.122699386503067</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>5.2044609665427503E-2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.122699386503067</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>5.65055762081784E-2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.122699386503067</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>6.0966542750929303E-2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.122699386503067</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>6.4684014869888395E-2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.12883435582822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>6.9144981412639403E-2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.12883435582822</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>7.2862453531598495E-2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.13496932515337401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>7.7323420074349405E-2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.13496932515337401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>8.1784386617100302E-2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.13496932515337401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>8.5501858736059394E-2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.14110429447852699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>8.9962825278810402E-2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.14110429447852699</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>9.3680297397769494E-2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.14723926380368099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>9.8141263940520404E-2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.14723926380368099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0.101115241635687</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.159509202453987</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>0.10334572490706299</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.17791411042944699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>0.10557620817843801</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.19631901840490701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0.109293680297397</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.20245398773006101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0.112267657992565</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.214723926380368</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>0.116728624535315</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.214723926380368</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0.121189591078066</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.214723926380368</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0.12416356877323401</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.22699386503067401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0.12788104089219299</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.23312883435582801</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>0.131598513011152</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.23926380368098099</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0.13457249070631899</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.251533742331288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>0.136802973977695</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.26993865030674802</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0.139776951672862</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.28220858895705497</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>0.14423791821561299</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.28220858895705497</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>0.147955390334572</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.28834355828220798</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>0.15018587360594701</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.306748466257668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>0.15315985130111501</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.31901840490797501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>0.15687732342007399</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.32515337423312801</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>0.15985130111524101</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.33742331288343502</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>0.16431226765799201</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.33742331288343502</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>0.16802973977695099</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.34355828220858797</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>0.17249070631970201</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.34355828220858797</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>0.176951672862453</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.34355828220858797</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>0.18066914498141201</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.34969325153374198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>0.185130111524163</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.34969325153374198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>0.18884758364312201</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.35582822085889498</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>0.19182156133828901</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.36809815950920199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>0.19628252788104</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.36809815950920199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>0.199256505576208</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.380368098159509</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>0.20297397769516701</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.38650306748466201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>0.20669144981412599</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.39263803680981502</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>0.21115241635687701</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.39263803680981502</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>0.215613382899628</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.39263803680981502</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>0.21933085501858701</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.39877300613496902</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>0.22304832713754599</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.40490797546012203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>0.226765799256505</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.41104294478527598</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>0.23048327137546401</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.41717791411042898</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>0.234944237918215</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.41717791411042898</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>0.239405204460966</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.41717791411042898</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>0.24237918215613299</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.42944785276073599</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>0.246096654275092</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.435582822085889</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>0.24981412639405201</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.441717791411042</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>0.25353159851301099</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.44785276073619601</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>0.25799256505576201</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.44785276073619601</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>0.26245353159851298</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.44785276073619601</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>0.26542750929367998</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.46012269938650302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>0.269888475836431</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.46012269938650302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>0.27360594795539001</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.46625766871165603</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>0.27732342007434901</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.47239263803680898</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>0.28178438661709998</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.47239263803680898</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>0.286245353159851</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.47239263803680898</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>0.29070631970260202</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.47239263803680898</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>0.29516728624535299</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.47239263803680898</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>0.29814126394051998</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.48466257668711599</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>0.30185873605947899</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.49079754601226899</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>0.30631970260223002</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.49079754601226899</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>0.31078066914498098</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.49079754601226899</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>0.31449814126393999</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.496932515337423</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>0.31895910780669101</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.496932515337423</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>0.32342007434944198</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.496932515337423</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>0.327881040892193</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.496932515337423</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>0.33159851301115201</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.503067484662576</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>0.33531598513011102</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.50920245398773001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>0.33977695167286198</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.50920245398773001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>0.344237918215613</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.50920245398773001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>0.34795539033457201</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.51533742331288301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>0.35167286245353102</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.52147239263803602</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>0.35613382899628199</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.52147239263803602</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>0.36059479553903301</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.52147239263803602</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>0.36282527881040799</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.53987730061349604</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>0.366542750929368</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.54601226993865004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>0.37026022304832701</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.55214723926380305</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>0.37397769516728602</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.55828220858895705</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>0.37843866171003698</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.55828220858895705</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>0.38066914498141202</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.57668711656441696</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>0.38438661710037098</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.58282208588956996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>0.388847583643122</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.58282208588956996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>0.39256505576208101</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.58895705521472397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>0.395539033457249</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.60122699386502998</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>0.398513011152416</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.61349693251533699</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>0.40297397769516702</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.61349693251533699</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>0.40594795539033401</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.625766871165644</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>0.40966542750929302</v>
+      </c>
+      <c r="B110" s="1">
+        <v>0.63190184049079701</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>0.41263940520446002</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.64417177914110402</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>0.41710037174721099</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.64417177914110402</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>0.42156133828996201</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.64417177914110402</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>0.42602230483271297</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.64417177914110402</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>0.43048327137546399</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0.64417177914110402</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>0.43345724907063199</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0.65644171779141103</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>0.437174721189591</v>
+      </c>
+      <c r="B117" s="1">
+        <v>0.66257668711656403</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>0.44163568773234202</v>
+      </c>
+      <c r="B118" s="1">
+        <v>0.66257668711656403</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>0.44609665427509199</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0.66257668711656403</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>0.45055762081784301</v>
+      </c>
+      <c r="B120" s="1">
+        <v>0.66257668711656403</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>0.45501858736059397</v>
+      </c>
+      <c r="B121" s="1">
+        <v>0.66257668711656403</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>0.45947955390334499</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0.66257668711656403</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>0.463197026022304</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0.66871165644171704</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>0.46691449814126301</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0.67484662576687104</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>0.47063197026022302</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0.68098159509202405</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>0.47434944237918197</v>
+      </c>
+      <c r="B126" s="1">
+        <v>0.68711656441717694</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>0.47657992565055701</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0.70552147239263796</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>0.48104089219330798</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0.70552147239263796</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>0.48475836431226699</v>
+      </c>
+      <c r="B129" s="1">
+        <v>0.71165644171779097</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>0.48921933085501801</v>
+      </c>
+      <c r="B130" s="1">
+        <v>0.71165644171779097</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>0.49293680297397702</v>
+      </c>
+      <c r="B131" s="1">
+        <v>0.71779141104294397</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>0.49739776951672798</v>
+      </c>
+      <c r="B132" s="1">
+        <v>0.71779141104294397</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>0.50037174721189503</v>
+      </c>
+      <c r="B133" s="1">
+        <v>0.73006134969325098</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>0.504832713754646</v>
+      </c>
+      <c r="B134" s="1">
+        <v>0.73006134969325098</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>0.50929368029739697</v>
+      </c>
+      <c r="B135" s="1">
+        <v>0.73006134969325098</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>0.51375464684014804</v>
+      </c>
+      <c r="B136" s="1">
+        <v>0.73006134969325098</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>0.51821561338289901</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0.73006134969325098</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>0.52193308550185802</v>
+      </c>
+      <c r="B138" s="1">
+        <v>0.73619631901840399</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>0.52565055762081703</v>
+      </c>
+      <c r="B139" s="1">
+        <v>0.74233128834355799</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>0.52936802973977604</v>
+      </c>
+      <c r="B140" s="1">
+        <v>0.748466257668711</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>0.533828996282527</v>
+      </c>
+      <c r="B141" s="1">
+        <v>0.748466257668711</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>0.53828996282527797</v>
+      </c>
+      <c r="B142" s="1">
+        <v>0.748466257668711</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>0.54275092936802904</v>
+      </c>
+      <c r="B143" s="1">
+        <v>0.748466257668711</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>0.54721189591078001</v>
+      </c>
+      <c r="B144" s="1">
+        <v>0.748466257668711</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>0.55092936802973902</v>
+      </c>
+      <c r="B145" s="1">
+        <v>0.754601226993865</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>0.55464684014869803</v>
+      </c>
+      <c r="B146" s="1">
+        <v>0.76073619631901801</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>0.55836431226765804</v>
+      </c>
+      <c r="B147" s="1">
+        <v>0.76687116564417102</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>0.562825278810408</v>
+      </c>
+      <c r="B148" s="1">
+        <v>0.76687116564417102</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>0.56728624535315897</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0.76687116564417102</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>0.57100371747211898</v>
+      </c>
+      <c r="B150" s="1">
+        <v>0.77300613496932502</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>0.57472118959107799</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0.77914110429447803</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>0.57918215613382895</v>
+      </c>
+      <c r="B152" s="1">
+        <v>0.77914110429447803</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>0.58289962825278796</v>
+      </c>
+      <c r="B153" s="1">
+        <v>0.78527607361963103</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>0.58736059479553904</v>
+      </c>
+      <c r="B154" s="1">
+        <v>0.78527607361963103</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>0.59182156133829</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0.78527607361963103</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>0.59553903345724901</v>
+      </c>
+      <c r="B156" s="1">
+        <v>0.79141104294478504</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>0.59925650557620802</v>
+      </c>
+      <c r="B157" s="1">
+        <v>0.79754601226993804</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>0.60297397769516703</v>
+      </c>
+      <c r="B158" s="1">
+        <v>0.80368098159509205</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>0.607434944237918</v>
+      </c>
+      <c r="B159" s="1">
+        <v>0.80368098159509205</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>0.61189591078066896</v>
+      </c>
+      <c r="B160" s="1">
+        <v>0.80368098159509205</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>0.61561338289962797</v>
+      </c>
+      <c r="B161" s="1">
+        <v>0.80981595092024505</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>0.61933085501858698</v>
+      </c>
+      <c r="B162" s="1">
+        <v>0.81595092024539795</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>0.62379182156133794</v>
+      </c>
+      <c r="B163" s="1">
+        <v>0.81595092024539795</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>0.62825278810408902</v>
+      </c>
+      <c r="B164" s="1">
+        <v>0.81595092024539795</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>0.63271375464683999</v>
+      </c>
+      <c r="B165" s="1">
+        <v>0.81595092024539795</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>0.636431226765799</v>
+      </c>
+      <c r="B166" s="1">
+        <v>0.82208588957055195</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>0.64089219330854996</v>
+      </c>
+      <c r="B167" s="1">
+        <v>0.82208588957055195</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>0.64535315985130104</v>
+      </c>
+      <c r="B168" s="1">
+        <v>0.82208588957055195</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>0.64981412639405201</v>
+      </c>
+      <c r="B169" s="1">
+        <v>0.82208588957055195</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>0.65353159851301101</v>
+      </c>
+      <c r="B170" s="1">
+        <v>0.82822085889570496</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>0.65724907063197002</v>
+      </c>
+      <c r="B171" s="1">
+        <v>0.83435582822085796</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>0.66171003717472099</v>
+      </c>
+      <c r="B172" s="1">
+        <v>0.83435582822085796</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>0.66542750929368</v>
+      </c>
+      <c r="B173" s="1">
+        <v>0.84049079754601197</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>0.66914498141263901</v>
+      </c>
+      <c r="B174" s="1">
+        <v>0.84662576687116498</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>0.67360594795538997</v>
+      </c>
+      <c r="B175" s="1">
+        <v>0.84662576687116498</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>0.67806691449814105</v>
+      </c>
+      <c r="B176" s="1">
+        <v>0.84662576687116498</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>0.68252788104089201</v>
+      </c>
+      <c r="B177" s="1">
+        <v>0.84662576687116498</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>0.68698884758364298</v>
+      </c>
+      <c r="B178" s="1">
+        <v>0.84662576687116498</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>0.69070631970260199</v>
+      </c>
+      <c r="B179" s="1">
+        <v>0.85276073619631898</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>0.694423791821561</v>
+      </c>
+      <c r="B180" s="1">
+        <v>0.85889570552147199</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>0.69888475836431196</v>
+      </c>
+      <c r="B181" s="1">
+        <v>0.85889570552147199</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>0.70334572490706304</v>
+      </c>
+      <c r="B182" s="1">
+        <v>0.85889570552147199</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>0.70780669144981401</v>
+      </c>
+      <c r="B183" s="1">
+        <v>0.85889570552147199</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>0.71226765799256497</v>
+      </c>
+      <c r="B184" s="1">
+        <v>0.85889570552147199</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>0.71598513011152398</v>
+      </c>
+      <c r="B185" s="1">
+        <v>0.86503067484662499</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>0.72044609665427495</v>
+      </c>
+      <c r="B186" s="1">
+        <v>0.86503067484662499</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>0.723420074349442</v>
+      </c>
+      <c r="B187" s="1">
+        <v>0.877300613496932</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>0.72788104089219297</v>
+      </c>
+      <c r="B188" s="1">
+        <v>0.877300613496932</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>0.73234200743494404</v>
+      </c>
+      <c r="B189" s="1">
+        <v>0.877300613496932</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>0.73680297397769501</v>
+      </c>
+      <c r="B190" s="1">
+        <v>0.877300613496932</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>0.73977695167286195</v>
+      </c>
+      <c r="B191" s="1">
+        <v>0.88957055214723901</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>0.74423791821561303</v>
+      </c>
+      <c r="B192" s="1">
+        <v>0.88957055214723901</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>0.74869888475836399</v>
+      </c>
+      <c r="B193" s="1">
+        <v>0.88957055214723901</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>0.75315985130111496</v>
+      </c>
+      <c r="B194" s="1">
+        <v>0.88957055214723901</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>0.75687732342007397</v>
+      </c>
+      <c r="B195" s="1">
+        <v>0.89570552147239202</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>0.76133828996282504</v>
+      </c>
+      <c r="B196" s="1">
+        <v>0.89570552147239202</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>0.76505576208178405</v>
+      </c>
+      <c r="B197" s="1">
+        <v>0.90184049079754602</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>0.76951672862453502</v>
+      </c>
+      <c r="B198" s="1">
+        <v>0.90184049079754602</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>0.77397769516728598</v>
+      </c>
+      <c r="B199" s="1">
+        <v>0.90184049079754602</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>0.77769516728624499</v>
+      </c>
+      <c r="B200" s="1">
+        <v>0.90797546012269903</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>0.781412639405204</v>
+      </c>
+      <c r="B201" s="1">
+        <v>0.91411042944785204</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>0.78587360594795497</v>
+      </c>
+      <c r="B202" s="1">
+        <v>0.91411042944785204</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>0.79033457249070604</v>
+      </c>
+      <c r="B203" s="1">
+        <v>0.91411042944785204</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>0.79479553903345701</v>
+      </c>
+      <c r="B204" s="1">
+        <v>0.91411042944785204</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>0.79925650557620798</v>
+      </c>
+      <c r="B205" s="1">
+        <v>0.91411042944785204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>0.80371747211895905</v>
+      </c>
+      <c r="B206" s="1">
+        <v>0.91411042944785204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>0.80743494423791795</v>
+      </c>
+      <c r="B207" s="1">
+        <v>0.92024539877300604</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>0.81189591078066903</v>
+      </c>
+      <c r="B208" s="1">
+        <v>0.92024539877300604</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>0.81635687732341999</v>
+      </c>
+      <c r="B209" s="1">
+        <v>0.92024539877300604</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>0.82081784386617096</v>
+      </c>
+      <c r="B210" s="1">
+        <v>0.92024539877300604</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>0.82527881040892104</v>
+      </c>
+      <c r="B211" s="1">
+        <v>0.92024539877300604</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>0.82899628252788105</v>
+      </c>
+      <c r="B212" s="1">
+        <v>0.92638036809815905</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>0.83345724907063201</v>
+      </c>
+      <c r="B213" s="1">
+        <v>0.92638036809815905</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>0.83717472118959102</v>
+      </c>
+      <c r="B214" s="1">
+        <v>0.93251533742331205</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>0.84163568773234199</v>
+      </c>
+      <c r="B215" s="1">
+        <v>0.93251533742331205</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>0.84609665427509295</v>
+      </c>
+      <c r="B216" s="1">
+        <v>0.93251533742331205</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>0.84981412639405196</v>
+      </c>
+      <c r="B217" s="1">
+        <v>0.93865030674846595</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>0.85427509293680204</v>
+      </c>
+      <c r="B218" s="1">
+        <v>0.93865030674846595</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>0.858736059479553</v>
+      </c>
+      <c r="B219" s="1">
+        <v>0.93865030674846595</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>0.86319702602230397</v>
+      </c>
+      <c r="B220" s="1">
+        <v>0.93865030674846595</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>0.86691449814126398</v>
+      </c>
+      <c r="B221" s="1">
+        <v>0.94478527607361895</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>0.87063197026022299</v>
+      </c>
+      <c r="B222" s="1">
+        <v>0.95092024539877296</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>0.874349442379182</v>
+      </c>
+      <c r="B223" s="1">
+        <v>0.95705521472392596</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>0.878066914498141</v>
+      </c>
+      <c r="B224" s="1">
+        <v>0.96319018404907897</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>0.88178438661710001</v>
+      </c>
+      <c r="B225" s="1">
+        <v>0.96932515337423297</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>0.88624535315985098</v>
+      </c>
+      <c r="B226" s="1">
+        <v>0.96932515337423297</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>0.89070631970260195</v>
+      </c>
+      <c r="B227" s="1">
+        <v>0.96932515337423297</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>0.89516728624535302</v>
+      </c>
+      <c r="B228" s="1">
+        <v>0.96932515337423297</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>0.89962825278810399</v>
+      </c>
+      <c r="B229" s="1">
+        <v>0.96932515337423297</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>0.903345724907063</v>
+      </c>
+      <c r="B230" s="1">
+        <v>0.97546012269938598</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>0.90780669144981396</v>
+      </c>
+      <c r="B231" s="1">
+        <v>0.97546012269938598</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>0.91226765799256504</v>
+      </c>
+      <c r="B232" s="1">
+        <v>0.97546012269938598</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>0.91672862453531601</v>
+      </c>
+      <c r="B233" s="1">
+        <v>0.97546012269938598</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>0.92118959107806597</v>
+      </c>
+      <c r="B234" s="1">
+        <v>0.97546012269938598</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>0.92565055762081705</v>
+      </c>
+      <c r="B235" s="1">
+        <v>0.97546012269938598</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>0.92936802973977695</v>
+      </c>
+      <c r="B236" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>0.93382899628252702</v>
+      </c>
+      <c r="B237" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>0.93828996282527799</v>
+      </c>
+      <c r="B238" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>0.94275092936802896</v>
+      </c>
+      <c r="B239" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>0.94721189591078003</v>
+      </c>
+      <c r="B240" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>0.951672862453531</v>
+      </c>
+      <c r="B241" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>0.95613382899628196</v>
+      </c>
+      <c r="B242" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>0.96059479553903304</v>
+      </c>
+      <c r="B243" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>0.96505576208178401</v>
+      </c>
+      <c r="B244" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>0.96951672862453497</v>
+      </c>
+      <c r="B245" s="1">
+        <v>0.98159509202453898</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>0.97323420074349398</v>
+      </c>
+      <c r="B246" s="1">
+        <v>0.98773006134969299</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>0.97769516728624495</v>
+      </c>
+      <c r="B247" s="1">
+        <v>0.98773006134969299</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>0.98215613382899603</v>
+      </c>
+      <c r="B248" s="1">
+        <v>0.98773006134969299</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>0.98661710037174699</v>
+      </c>
+      <c r="B249" s="1">
+        <v>0.98773006134969299</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>0.98959107806691404</v>
+      </c>
+      <c r="B250" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>0.99405204460966501</v>
+      </c>
+      <c r="B251" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>0.99851301115241597</v>
+      </c>
+      <c r="B252" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>1</v>
+      </c>
+      <c r="B253" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>